<commit_message>
OR and Script updated
Files update
</commit_message>
<xml_diff>
--- a/TestData/JTPS-DEVQA/ChargeIntervalTypes.xlsx
+++ b/TestData/JTPS-DEVQA/ChargeIntervalTypes.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="116">
   <si>
     <t>EOF</t>
   </si>
@@ -380,9 +380,6 @@
     <t>elm_Close</t>
   </si>
   <si>
-    <t>wind_ChargeIntervalTypes</t>
-  </si>
-  <si>
     <t>allrows,value^zxy</t>
   </si>
   <si>
@@ -396,6 +393,9 @@
   </si>
   <si>
     <t>Charge Interval Types</t>
+  </si>
+  <si>
+    <t>wnd_ChargeIntervalTypes</t>
   </si>
 </sst>
 </file>
@@ -1013,17 +1013,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:X86"/>
+  <dimension ref="A1:X88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="G40" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1037,7 +1037,8 @@
     <col min="14" max="14" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.85546875" style="1" customWidth="1"/>
-    <col min="17" max="21" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.7109375" style="1" customWidth="1"/>
+    <col min="18" max="21" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -1126,7 +1127,7 @@
         <v>106</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="7" t="s">
@@ -1176,7 +1177,7 @@
         <v>106</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="7" t="s">
@@ -1457,7 +1458,7 @@
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>3</v>
@@ -1524,7 +1525,7 @@
       <c r="X10" s="2"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="2"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1532,7 +1533,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>7</v>
@@ -1541,12 +1542,12 @@
         <v>6</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10" t="s">
-        <v>4</v>
+        <v>53</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="18">
+        <v>2</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>3</v>
@@ -1554,23 +1555,18 @@
       <c r="N11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P11" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="3"/>
+      <c r="O11" s="32"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="2"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="2"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1578,7 +1574,7 @@
         <v>7</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>7</v>
@@ -1587,29 +1583,33 @@
         <v>6</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="18">
+        <v>24</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P12" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O12" s="21"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="30"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="2"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -1620,7 +1620,7 @@
         <v>7</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>7</v>
@@ -1631,42 +1631,40 @@
       <c r="I13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="18" t="s">
-        <v>114</v>
-      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
       <c r="M13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P13" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
+      <c r="O13" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-      <c r="X13" s="30"/>
+      <c r="X13" s="3"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="13"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>7</v>
@@ -1675,12 +1673,12 @@
         <v>6</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="18" t="s">
-        <v>21</v>
+        <v>53</v>
+      </c>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="18">
+        <v>1</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>3</v>
@@ -1688,31 +1686,27 @@
       <c r="N14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="X14" s="30"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
+      <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="8"/>
       <c r="E15" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>7</v>
@@ -1721,12 +1715,12 @@
         <v>6</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="31" t="s">
-        <v>23</v>
+      <c r="L15" s="18" t="s">
+        <v>113</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>3</v>
@@ -1734,17 +1728,17 @@
       <c r="N15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O15" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P15" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
+      <c r="O15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P15" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="30"/>
@@ -1753,12 +1747,12 @@
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>7</v>
@@ -1767,12 +1761,12 @@
         <v>6</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="12" t="s">
-        <v>23</v>
+        <v>5</v>
+      </c>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>3</v>
@@ -1780,31 +1774,31 @@
       <c r="N16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O16" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P16" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
+      <c r="O16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
-      <c r="X16" s="9"/>
+      <c r="X16" s="30"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="13"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="13"/>
       <c r="E17" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>7</v>
@@ -1817,7 +1811,7 @@
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="12" t="s">
+      <c r="L17" s="31" t="s">
         <v>23</v>
       </c>
       <c r="M17" s="3" t="s">
@@ -1827,10 +1821,10 @@
         <v>2</v>
       </c>
       <c r="O17" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
@@ -1839,18 +1833,18 @@
       <c r="U17" s="10"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
-      <c r="X17" s="9"/>
+      <c r="X17" s="30"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>7</v>
@@ -1859,12 +1853,12 @@
         <v>6</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="14" t="s">
-        <v>111</v>
+      <c r="L18" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>3</v>
@@ -1873,10 +1867,10 @@
         <v>2</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P18" s="11" t="s">
-        <v>14</v>
+        <v>115</v>
+      </c>
+      <c r="P18" s="28" t="s">
+        <v>13</v>
       </c>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
@@ -1896,7 +1890,7 @@
         <v>7</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>7</v>
@@ -1905,12 +1899,12 @@
         <v>6</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="12" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="M19" s="3" t="s">
         <v>3</v>
@@ -1919,10 +1913,10 @@
         <v>2</v>
       </c>
       <c r="O19" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P19" s="11" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
@@ -1942,7 +1936,7 @@
         <v>7</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>7</v>
@@ -1951,12 +1945,12 @@
         <v>6</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="18">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="M20" s="3" t="s">
         <v>3</v>
@@ -1964,8 +1958,12 @@
       <c r="N20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O20" s="32"/>
-      <c r="P20" s="11"/>
+      <c r="O20" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P20" s="11" t="s">
+        <v>14</v>
+      </c>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
@@ -1995,6 +1993,7 @@
       <c r="I21" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="12" t="s">
         <v>4</v>
@@ -2005,11 +2004,11 @@
       <c r="N21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O21" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="P21" s="3" t="s">
-        <v>107</v>
+      <c r="O21" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P21" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
@@ -2029,7 +2028,7 @@
         <v>7</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>7</v>
@@ -2038,12 +2037,12 @@
         <v>6</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="12" t="s">
-        <v>4</v>
+        <v>53</v>
+      </c>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="18">
+        <v>1</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>3</v>
@@ -2051,12 +2050,8 @@
       <c r="N22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O22" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P22" s="11" t="s">
-        <v>9</v>
-      </c>
+      <c r="O22" s="32"/>
+      <c r="P22" s="11"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
@@ -2069,13 +2064,13 @@
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="8"/>
+      <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>7</v>
@@ -2084,12 +2079,11 @@
         <v>6</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J23" s="3"/>
+        <v>5</v>
+      </c>
       <c r="K23" s="3"/>
       <c r="L23" s="12" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>3</v>
@@ -2097,10 +2091,12 @@
       <c r="N23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O23" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P23" s="11"/>
+      <c r="O23" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
@@ -2113,13 +2109,13 @@
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="8"/>
+      <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>7</v>
@@ -2128,12 +2124,12 @@
         <v>6</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="12" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="M24" s="3" t="s">
         <v>3</v>
@@ -2142,10 +2138,10 @@
         <v>2</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P24" s="28" t="s">
-        <v>50</v>
+        <v>115</v>
+      </c>
+      <c r="P24" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="Q24" s="10"/>
       <c r="R24" s="10"/>
@@ -2165,7 +2161,7 @@
         <v>7</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>7</v>
@@ -2188,11 +2184,9 @@
         <v>2</v>
       </c>
       <c r="O25" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P25" s="11" t="s">
-        <v>59</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="P25" s="11"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
@@ -2200,7 +2194,7 @@
       <c r="U25" s="10"/>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
-      <c r="X25" s="3"/>
+      <c r="X25" s="9"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
@@ -2220,12 +2214,12 @@
         <v>6</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="12" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="M26" s="3" t="s">
         <v>3</v>
@@ -2234,10 +2228,10 @@
         <v>2</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P26" s="11" t="s">
-        <v>58</v>
+        <v>115</v>
+      </c>
+      <c r="P26" s="28" t="s">
+        <v>50</v>
       </c>
       <c r="Q26" s="10"/>
       <c r="R26" s="10"/>
@@ -2246,12 +2240,12 @@
       <c r="U26" s="10"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
-      <c r="X26" s="3"/>
+      <c r="X26" s="9"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="13"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="8"/>
       <c r="D27" s="13"/>
       <c r="E27" s="7" t="s">
         <v>7</v>
@@ -2280,10 +2274,10 @@
         <v>2</v>
       </c>
       <c r="O27" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P27" s="11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
@@ -2303,7 +2297,7 @@
         <v>7</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>7</v>
@@ -2312,12 +2306,12 @@
         <v>6</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="12" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>3</v>
@@ -2326,10 +2320,10 @@
         <v>2</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P28" s="28" t="s">
-        <v>50</v>
+        <v>115</v>
+      </c>
+      <c r="P28" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
@@ -2338,18 +2332,18 @@
       <c r="U28" s="10"/>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
-      <c r="X28" s="9"/>
+      <c r="X28" s="3"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="8"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>7</v>
@@ -2358,12 +2352,12 @@
         <v>6</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="18">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="M29" s="3" t="s">
         <v>3</v>
@@ -2371,16 +2365,20 @@
       <c r="N29" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O29" s="21"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="21"/>
-      <c r="S29" s="21"/>
-      <c r="T29" s="21"/>
-      <c r="U29" s="21"/>
+      <c r="O29" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P29" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
-      <c r="X29" s="9"/>
+      <c r="X29" s="3"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -2405,7 +2403,7 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="12" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="M30" s="3" t="s">
         <v>3</v>
@@ -2414,7 +2412,7 @@
         <v>2</v>
       </c>
       <c r="O30" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P30" s="28" t="s">
         <v>50</v>
@@ -2433,25 +2431,25 @@
       <c r="B31" s="2"/>
       <c r="C31" s="8"/>
       <c r="D31" s="13"/>
-      <c r="E31" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="I31" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="12" t="s">
-        <v>4</v>
+      <c r="E31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="18">
+        <v>1</v>
       </c>
       <c r="M31" s="3" t="s">
         <v>3</v>
@@ -2459,45 +2457,41 @@
       <c r="N31" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O31" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="P31" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q31" s="23"/>
-      <c r="R31" s="23"/>
-      <c r="S31" s="23"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="23"/>
-      <c r="V31" s="22"/>
-      <c r="W31" s="22"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
       <c r="X31" s="9"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="13"/>
+      <c r="C32" s="8"/>
       <c r="D32" s="13"/>
-      <c r="E32" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="F32" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="I32" s="25" t="s">
-        <v>48</v>
+      <c r="E32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="15" t="s">
-        <v>47</v>
+      <c r="L32" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="M32" s="3" t="s">
         <v>3</v>
@@ -2505,20 +2499,20 @@
       <c r="N32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O32" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="P32" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="22"/>
-      <c r="W32" s="22"/>
-      <c r="X32" s="3"/>
+      <c r="O32" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P32" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="9"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -2529,7 +2523,7 @@
         <v>46</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G33" s="27" t="s">
         <v>7</v>
@@ -2537,18 +2531,26 @@
       <c r="H33" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I33" s="25"/>
+      <c r="I33" s="25" t="s">
+        <v>5</v>
+      </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
-      <c r="L33" s="12"/>
+      <c r="L33" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="M33" s="3" t="s">
         <v>3</v>
       </c>
       <c r="N33" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O33" s="23"/>
-      <c r="P33" s="24"/>
+      <c r="O33" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="P33" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="Q33" s="23"/>
       <c r="R33" s="23"/>
       <c r="S33" s="23"/>
@@ -2556,34 +2558,32 @@
       <c r="U33" s="23"/>
       <c r="V33" s="22"/>
       <c r="W33" s="22"/>
-      <c r="X33" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="X33" s="9"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
-      <c r="E34" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>5</v>
+      <c r="E34" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" s="25" t="s">
+        <v>48</v>
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
-      <c r="L34" s="12" t="s">
-        <v>4</v>
+      <c r="L34" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="M34" s="3" t="s">
         <v>3</v>
@@ -2591,66 +2591,60 @@
       <c r="N34" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O34" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P34" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="10"/>
-      <c r="T34" s="10"/>
-      <c r="U34" s="10"/>
-      <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
-      <c r="X34" s="9"/>
+      <c r="O34" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="P34" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="23"/>
+      <c r="S34" s="23"/>
+      <c r="T34" s="23"/>
+      <c r="U34" s="23"/>
+      <c r="V34" s="22"/>
+      <c r="W34" s="22"/>
+      <c r="X34" s="3"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="13"/>
+      <c r="C35" s="8"/>
       <c r="D35" s="13"/>
-      <c r="E35" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="E35" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" s="25"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="12" t="s">
-        <v>42</v>
-      </c>
+      <c r="L35" s="12"/>
       <c r="M35" s="3" t="s">
         <v>3</v>
       </c>
       <c r="N35" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O35" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P35" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="10"/>
-      <c r="T35" s="10"/>
-      <c r="U35" s="10"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="2"/>
-      <c r="X35" s="9"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
+      <c r="S35" s="23"/>
+      <c r="T35" s="23"/>
+      <c r="U35" s="23"/>
+      <c r="V35" s="22"/>
+      <c r="W35" s="22"/>
+      <c r="X35" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
@@ -2661,7 +2655,7 @@
         <v>7</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>7</v>
@@ -2674,8 +2668,8 @@
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="19" t="s">
-        <v>112</v>
+      <c r="L36" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="M36" s="3" t="s">
         <v>3</v>
@@ -2684,10 +2678,10 @@
         <v>2</v>
       </c>
       <c r="O36" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P36" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q36" s="10"/>
       <c r="R36" s="10"/>
@@ -2707,7 +2701,7 @@
         <v>7</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>7</v>
@@ -2730,10 +2724,10 @@
         <v>2</v>
       </c>
       <c r="O37" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P37" s="11" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="Q37" s="10"/>
       <c r="R37" s="10"/>
@@ -2753,7 +2747,7 @@
         <v>7</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>7</v>
@@ -2766,8 +2760,8 @@
       </c>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="12" t="s">
-        <v>4</v>
+      <c r="L38" s="19" t="s">
+        <v>111</v>
       </c>
       <c r="M38" s="3" t="s">
         <v>3</v>
@@ -2776,10 +2770,10 @@
         <v>2</v>
       </c>
       <c r="O38" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P38" s="11" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="Q38" s="10"/>
       <c r="R38" s="10"/>
@@ -2793,13 +2787,13 @@
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="8"/>
+      <c r="C39" s="13"/>
       <c r="D39" s="13"/>
       <c r="E39" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>7</v>
@@ -2808,12 +2802,12 @@
         <v>6</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="12" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="M39" s="3" t="s">
         <v>3</v>
@@ -2822,9 +2816,11 @@
         <v>2</v>
       </c>
       <c r="O39" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P39" s="11"/>
+        <v>115</v>
+      </c>
+      <c r="P39" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="Q39" s="10"/>
       <c r="R39" s="10"/>
       <c r="S39" s="10"/>
@@ -2832,7 +2828,7 @@
       <c r="U39" s="10"/>
       <c r="V39" s="2"/>
       <c r="W39" s="2"/>
-      <c r="X39" s="3"/>
+      <c r="X39" s="9"/>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
@@ -2843,7 +2839,7 @@
         <v>7</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>7</v>
@@ -2852,12 +2848,12 @@
         <v>6</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="12" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="M40" s="3" t="s">
         <v>3</v>
@@ -2866,10 +2862,10 @@
         <v>2</v>
       </c>
       <c r="O40" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P40" s="11" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="Q40" s="10"/>
       <c r="R40" s="10"/>
@@ -2883,13 +2879,13 @@
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="13"/>
+      <c r="C41" s="8"/>
       <c r="D41" s="13"/>
       <c r="E41" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>7</v>
@@ -2898,12 +2894,12 @@
         <v>6</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="12" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="M41" s="3" t="s">
         <v>3</v>
@@ -2912,11 +2908,9 @@
         <v>2</v>
       </c>
       <c r="O41" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P41" s="11" t="s">
-        <v>1</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="P41" s="11"/>
       <c r="Q41" s="10"/>
       <c r="R41" s="10"/>
       <c r="S41" s="10"/>
@@ -2924,7 +2918,7 @@
       <c r="U41" s="10"/>
       <c r="V41" s="2"/>
       <c r="W41" s="2"/>
-      <c r="X41" s="9"/>
+      <c r="X41" s="3"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
@@ -2944,12 +2938,12 @@
         <v>6</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J42" s="17"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="18" t="s">
-        <v>114</v>
+        <v>24</v>
+      </c>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="M42" s="3" t="s">
         <v>3</v>
@@ -2957,23 +2951,23 @@
       <c r="N42" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P42" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
+      <c r="O42" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P42" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
       <c r="X42" s="9"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
+      <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
@@ -2981,7 +2975,7 @@
         <v>7</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>7</v>
@@ -2994,8 +2988,8 @@
       </c>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
-      <c r="L43" s="17" t="s">
-        <v>21</v>
+      <c r="L43" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="M43" s="3" t="s">
         <v>3</v>
@@ -3003,22 +2997,22 @@
       <c r="N43" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O43" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P43" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q43" s="3"/>
-      <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
+      <c r="O43" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P43" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="10"/>
       <c r="V43" s="2"/>
       <c r="W43" s="2"/>
       <c r="X43" s="9"/>
     </row>
-    <row r="44" spans="1:24" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="13"/>
@@ -3027,7 +3021,7 @@
         <v>7</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>7</v>
@@ -3036,11 +3030,11 @@
         <v>6</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="18" t="s">
         <v>113</v>
       </c>
       <c r="M44" s="3" t="s">
@@ -3049,23 +3043,23 @@
       <c r="N44" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O44" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P44" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="S44" s="10"/>
-      <c r="T44" s="10"/>
-      <c r="U44" s="10"/>
-      <c r="V44" s="20"/>
-      <c r="W44" s="20"/>
+      <c r="O44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P44" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
       <c r="X44" s="9"/>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="2"/>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
@@ -3073,7 +3067,7 @@
         <v>7</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>7</v>
@@ -3086,8 +3080,8 @@
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
-      <c r="L45" s="12" t="s">
-        <v>4</v>
+      <c r="L45" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="M45" s="3" t="s">
         <v>3</v>
@@ -3095,22 +3089,22 @@
       <c r="N45" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O45" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P45" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q45" s="10"/>
-      <c r="R45" s="10"/>
-      <c r="S45" s="10"/>
-      <c r="T45" s="10"/>
-      <c r="U45" s="10"/>
-      <c r="V45" s="20"/>
-      <c r="W45" s="20"/>
+      <c r="O45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P45" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+      <c r="U45" s="3"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
       <c r="X45" s="9"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="13"/>
@@ -3119,7 +3113,7 @@
         <v>7</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>7</v>
@@ -3128,12 +3122,12 @@
         <v>6</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J46" s="17"/>
-      <c r="K46" s="17"/>
-      <c r="L46" s="18" t="s">
-        <v>114</v>
+        <v>18</v>
+      </c>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="14" t="s">
+        <v>112</v>
       </c>
       <c r="M46" s="3" t="s">
         <v>3</v>
@@ -3141,11 +3135,11 @@
       <c r="N46" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O46" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P46" s="16" t="s">
-        <v>19</v>
+      <c r="O46" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P46" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="Q46" s="10"/>
       <c r="R46" s="10"/>
@@ -3165,7 +3159,7 @@
         <v>7</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>7</v>
@@ -3178,8 +3172,8 @@
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
-      <c r="L47" s="17" t="s">
-        <v>21</v>
+      <c r="L47" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="M47" s="3" t="s">
         <v>3</v>
@@ -3187,11 +3181,11 @@
       <c r="N47" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O47" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P47" s="16" t="s">
-        <v>19</v>
+      <c r="O47" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P47" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="Q47" s="10"/>
       <c r="R47" s="10"/>
@@ -3205,13 +3199,13 @@
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="8"/>
+      <c r="C48" s="13"/>
       <c r="D48" s="13"/>
       <c r="E48" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>7</v>
@@ -3222,10 +3216,10 @@
       <c r="I48" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="12" t="s">
-        <v>4</v>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="18" t="s">
+        <v>113</v>
       </c>
       <c r="M48" s="3" t="s">
         <v>3</v>
@@ -3233,20 +3227,20 @@
       <c r="N48" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O48" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P48" s="11" t="s">
-        <v>32</v>
+      <c r="O48" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P48" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="Q48" s="10"/>
       <c r="R48" s="10"/>
       <c r="S48" s="10"/>
       <c r="T48" s="10"/>
       <c r="U48" s="10"/>
-      <c r="V48" s="2"/>
-      <c r="W48" s="2"/>
-      <c r="X48" s="3"/>
+      <c r="V48" s="20"/>
+      <c r="W48" s="20"/>
+      <c r="X48" s="9"/>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
@@ -3257,7 +3251,7 @@
         <v>7</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>7</v>
@@ -3270,8 +3264,8 @@
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
-      <c r="L49" s="12" t="s">
-        <v>37</v>
+      <c r="L49" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="M49" s="3" t="s">
         <v>3</v>
@@ -3279,31 +3273,31 @@
       <c r="N49" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O49" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P49" s="11" t="s">
-        <v>16</v>
+      <c r="O49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P49" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="Q49" s="10"/>
       <c r="R49" s="10"/>
       <c r="S49" s="10"/>
       <c r="T49" s="10"/>
       <c r="U49" s="10"/>
-      <c r="V49" s="2"/>
-      <c r="W49" s="2"/>
-      <c r="X49" s="3"/>
+      <c r="V49" s="20"/>
+      <c r="W49" s="20"/>
+      <c r="X49" s="9"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
-      <c r="C50" s="13"/>
+      <c r="C50" s="8"/>
       <c r="D50" s="13"/>
       <c r="E50" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>7</v>
@@ -3316,8 +3310,8 @@
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
-      <c r="L50" s="19" t="s">
-        <v>112</v>
+      <c r="L50" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="M50" s="3" t="s">
         <v>3</v>
@@ -3326,10 +3320,10 @@
         <v>2</v>
       </c>
       <c r="O50" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P50" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q50" s="10"/>
       <c r="R50" s="10"/>
@@ -3349,7 +3343,7 @@
         <v>7</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>7</v>
@@ -3372,10 +3366,10 @@
         <v>2</v>
       </c>
       <c r="O51" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P51" s="11" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="Q51" s="10"/>
       <c r="R51" s="10"/>
@@ -3395,7 +3389,7 @@
         <v>7</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>7</v>
@@ -3408,8 +3402,8 @@
       </c>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
-      <c r="L52" s="12" t="s">
-        <v>4</v>
+      <c r="L52" s="19" t="s">
+        <v>111</v>
       </c>
       <c r="M52" s="3" t="s">
         <v>3</v>
@@ -3418,10 +3412,10 @@
         <v>2</v>
       </c>
       <c r="O52" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P52" s="11" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="Q52" s="10"/>
       <c r="R52" s="10"/>
@@ -3432,7 +3426,7 @@
       <c r="W52" s="2"/>
       <c r="X52" s="3"/>
     </row>
-    <row r="53" spans="1:24" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="13"/>
@@ -3441,7 +3435,7 @@
         <v>7</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>7</v>
@@ -3450,12 +3444,12 @@
         <v>6</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M53" s="3" t="s">
         <v>3</v>
@@ -3464,10 +3458,10 @@
         <v>2</v>
       </c>
       <c r="O53" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P53" s="11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q53" s="10"/>
       <c r="R53" s="10"/>
@@ -3487,7 +3481,7 @@
         <v>7</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="G54" s="6" t="s">
         <v>7</v>
@@ -3510,10 +3504,10 @@
         <v>2</v>
       </c>
       <c r="O54" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P54" s="11" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="Q54" s="10"/>
       <c r="R54" s="10"/>
@@ -3524,7 +3518,7 @@
       <c r="W54" s="2"/>
       <c r="X54" s="3"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="13"/>
@@ -3533,7 +3527,7 @@
         <v>7</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G55" s="6" t="s">
         <v>7</v>
@@ -3542,12 +3536,12 @@
         <v>6</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17"/>
-      <c r="L55" s="18" t="s">
-        <v>114</v>
+        <v>24</v>
+      </c>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="M55" s="3" t="s">
         <v>3</v>
@@ -3555,17 +3549,17 @@
       <c r="N55" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O55" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P55" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="3"/>
-      <c r="S55" s="3"/>
-      <c r="T55" s="3"/>
-      <c r="U55" s="3"/>
+      <c r="O55" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P55" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q55" s="10"/>
+      <c r="R55" s="10"/>
+      <c r="S55" s="10"/>
+      <c r="T55" s="10"/>
+      <c r="U55" s="10"/>
       <c r="V55" s="2"/>
       <c r="W55" s="2"/>
       <c r="X55" s="3"/>
@@ -3579,7 +3573,7 @@
         <v>7</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G56" s="6" t="s">
         <v>7</v>
@@ -3592,8 +3586,8 @@
       </c>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
-      <c r="L56" s="17" t="s">
-        <v>21</v>
+      <c r="L56" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="M56" s="3" t="s">
         <v>3</v>
@@ -3601,17 +3595,17 @@
       <c r="N56" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O56" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P56" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q56" s="3"/>
-      <c r="R56" s="3"/>
-      <c r="S56" s="3"/>
-      <c r="T56" s="3"/>
-      <c r="U56" s="3"/>
+      <c r="O56" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P56" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="10"/>
+      <c r="R56" s="10"/>
+      <c r="S56" s="10"/>
+      <c r="T56" s="10"/>
+      <c r="U56" s="10"/>
       <c r="V56" s="2"/>
       <c r="W56" s="2"/>
       <c r="X56" s="3"/>
@@ -3625,7 +3619,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>7</v>
@@ -3636,10 +3630,10 @@
       <c r="I57" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="12" t="s">
-        <v>4</v>
+      <c r="J57" s="17"/>
+      <c r="K57" s="17"/>
+      <c r="L57" s="18" t="s">
+        <v>113</v>
       </c>
       <c r="M57" s="3" t="s">
         <v>3</v>
@@ -3647,17 +3641,17 @@
       <c r="N57" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O57" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P57" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q57" s="10"/>
-      <c r="R57" s="10"/>
-      <c r="S57" s="10"/>
-      <c r="T57" s="10"/>
-      <c r="U57" s="10"/>
+      <c r="O57" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P57" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="3"/>
+      <c r="T57" s="3"/>
+      <c r="U57" s="3"/>
       <c r="V57" s="2"/>
       <c r="W57" s="2"/>
       <c r="X57" s="3"/>
@@ -3671,7 +3665,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>7</v>
@@ -3680,12 +3674,12 @@
         <v>6</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
-      <c r="L58" s="12">
-        <v>1</v>
+      <c r="L58" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="M58" s="3" t="s">
         <v>3</v>
@@ -3693,13 +3687,17 @@
       <c r="N58" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O58" s="10"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="10"/>
-      <c r="R58" s="10"/>
-      <c r="S58" s="10"/>
-      <c r="T58" s="10"/>
-      <c r="U58" s="10"/>
+      <c r="O58" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P58" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
       <c r="V58" s="2"/>
       <c r="W58" s="2"/>
       <c r="X58" s="3"/>
@@ -3713,7 +3711,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G59" s="6" t="s">
         <v>7</v>
@@ -3736,10 +3734,10 @@
         <v>2</v>
       </c>
       <c r="O59" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P59" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q59" s="10"/>
       <c r="R59" s="10"/>
@@ -3759,7 +3757,7 @@
         <v>7</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G60" s="6" t="s">
         <v>7</v>
@@ -3768,12 +3766,12 @@
         <v>6</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
-      <c r="L60" s="19" t="s">
-        <v>108</v>
+      <c r="L60" s="12">
+        <v>1</v>
       </c>
       <c r="M60" s="3" t="s">
         <v>3</v>
@@ -3781,12 +3779,8 @@
       <c r="N60" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O60" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P60" s="11" t="s">
-        <v>31</v>
-      </c>
+      <c r="O60" s="10"/>
+      <c r="P60" s="11"/>
       <c r="Q60" s="10"/>
       <c r="R60" s="10"/>
       <c r="S60" s="10"/>
@@ -3805,10 +3799,10 @@
         <v>7</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>6</v>
@@ -3828,10 +3822,10 @@
         <v>2</v>
       </c>
       <c r="O61" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P61" s="11" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="Q61" s="10"/>
       <c r="R61" s="10"/>
@@ -3851,7 +3845,7 @@
         <v>7</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>7</v>
@@ -3860,12 +3854,12 @@
         <v>6</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
-      <c r="L62" s="15" t="s">
-        <v>23</v>
+      <c r="L62" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="M62" s="3" t="s">
         <v>3</v>
@@ -3874,10 +3868,10 @@
         <v>2</v>
       </c>
       <c r="O62" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P62" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q62" s="10"/>
       <c r="R62" s="10"/>
@@ -3897,7 +3891,7 @@
         <v>7</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G63" s="6" t="s">
         <v>7</v>
@@ -3906,12 +3900,12 @@
         <v>6</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
-      <c r="L63" s="15" t="s">
-        <v>23</v>
+      <c r="L63" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="M63" s="3" t="s">
         <v>3</v>
@@ -3920,10 +3914,10 @@
         <v>2</v>
       </c>
       <c r="O63" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P63" s="11" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="Q63" s="10"/>
       <c r="R63" s="10"/>
@@ -3943,7 +3937,7 @@
         <v>7</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="G64" s="6" t="s">
         <v>7</v>
@@ -3952,12 +3946,12 @@
         <v>6</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
-      <c r="L64" s="12" t="s">
-        <v>4</v>
+      <c r="L64" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="M64" s="3" t="s">
         <v>3</v>
@@ -3966,10 +3960,10 @@
         <v>2</v>
       </c>
       <c r="O64" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P64" s="11" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="Q64" s="10"/>
       <c r="R64" s="10"/>
@@ -3989,7 +3983,7 @@
         <v>7</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>7</v>
@@ -3998,12 +3992,12 @@
         <v>6</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
-      <c r="L65" s="18" t="s">
-        <v>114</v>
+      <c r="L65" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="M65" s="3" t="s">
         <v>3</v>
@@ -4011,17 +4005,17 @@
       <c r="N65" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O65" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P65" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q65" s="3"/>
-      <c r="R65" s="3"/>
-      <c r="S65" s="3"/>
-      <c r="T65" s="3"/>
-      <c r="U65" s="3"/>
+      <c r="O65" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P65" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q65" s="10"/>
+      <c r="R65" s="10"/>
+      <c r="S65" s="10"/>
+      <c r="T65" s="10"/>
+      <c r="U65" s="10"/>
       <c r="V65" s="2"/>
       <c r="W65" s="2"/>
       <c r="X65" s="3"/>
@@ -4035,7 +4029,7 @@
         <v>7</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G66" s="6" t="s">
         <v>7</v>
@@ -4048,8 +4042,8 @@
       </c>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
-      <c r="L66" s="17" t="s">
-        <v>21</v>
+      <c r="L66" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="M66" s="3" t="s">
         <v>3</v>
@@ -4057,17 +4051,17 @@
       <c r="N66" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O66" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P66" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q66" s="3"/>
-      <c r="R66" s="3"/>
-      <c r="S66" s="3"/>
-      <c r="T66" s="3"/>
-      <c r="U66" s="3"/>
+      <c r="O66" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P66" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="10"/>
+      <c r="R66" s="10"/>
+      <c r="S66" s="10"/>
+      <c r="T66" s="10"/>
+      <c r="U66" s="10"/>
       <c r="V66" s="2"/>
       <c r="W66" s="2"/>
       <c r="X66" s="3"/>
@@ -4081,7 +4075,7 @@
         <v>7</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>7</v>
@@ -4094,8 +4088,8 @@
       </c>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
-      <c r="L67" s="15" t="s">
-        <v>25</v>
+      <c r="L67" s="18" t="s">
+        <v>113</v>
       </c>
       <c r="M67" s="3" t="s">
         <v>3</v>
@@ -4103,17 +4097,17 @@
       <c r="N67" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O67" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P67" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q67" s="10"/>
-      <c r="R67" s="10"/>
-      <c r="S67" s="10"/>
-      <c r="T67" s="10"/>
-      <c r="U67" s="10"/>
+      <c r="O67" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P67" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="3"/>
       <c r="V67" s="2"/>
       <c r="W67" s="2"/>
       <c r="X67" s="3"/>
@@ -4121,13 +4115,13 @@
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
-      <c r="C68" s="8"/>
+      <c r="C68" s="13"/>
       <c r="D68" s="13"/>
       <c r="E68" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>7</v>
@@ -4140,8 +4134,8 @@
       </c>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
-      <c r="L68" s="12" t="s">
-        <v>4</v>
+      <c r="L68" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="M68" s="3" t="s">
         <v>3</v>
@@ -4149,17 +4143,17 @@
       <c r="N68" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O68" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P68" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q68" s="10"/>
-      <c r="R68" s="10"/>
-      <c r="S68" s="10"/>
-      <c r="T68" s="10"/>
-      <c r="U68" s="10"/>
+      <c r="O68" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P68" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="3"/>
+      <c r="T68" s="3"/>
+      <c r="U68" s="3"/>
       <c r="V68" s="2"/>
       <c r="W68" s="2"/>
       <c r="X68" s="3"/>
@@ -4173,7 +4167,7 @@
         <v>7</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G69" s="6" t="s">
         <v>7</v>
@@ -4182,12 +4176,12 @@
         <v>6</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
       <c r="L69" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M69" s="3" t="s">
         <v>3</v>
@@ -4196,14 +4190,16 @@
         <v>2</v>
       </c>
       <c r="O69" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P69" s="10"/>
-      <c r="Q69" s="3"/>
-      <c r="R69" s="3"/>
-      <c r="S69" s="3"/>
-      <c r="T69" s="3"/>
-      <c r="U69" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="P69" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q69" s="10"/>
+      <c r="R69" s="10"/>
+      <c r="S69" s="10"/>
+      <c r="T69" s="10"/>
+      <c r="U69" s="10"/>
       <c r="V69" s="2"/>
       <c r="W69" s="2"/>
       <c r="X69" s="3"/>
@@ -4211,13 +4207,13 @@
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
-      <c r="C70" s="13"/>
+      <c r="C70" s="8"/>
       <c r="D70" s="13"/>
       <c r="E70" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G70" s="6" t="s">
         <v>7</v>
@@ -4230,8 +4226,8 @@
       </c>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
-      <c r="L70" s="18" t="s">
-        <v>114</v>
+      <c r="L70" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="M70" s="3" t="s">
         <v>3</v>
@@ -4239,17 +4235,17 @@
       <c r="N70" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O70" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P70" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q70" s="3"/>
-      <c r="R70" s="3"/>
-      <c r="S70" s="3"/>
-      <c r="T70" s="3"/>
-      <c r="U70" s="3"/>
+      <c r="O70" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P70" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q70" s="10"/>
+      <c r="R70" s="10"/>
+      <c r="S70" s="10"/>
+      <c r="T70" s="10"/>
+      <c r="U70" s="10"/>
       <c r="V70" s="2"/>
       <c r="W70" s="2"/>
       <c r="X70" s="3"/>
@@ -4263,7 +4259,7 @@
         <v>7</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G71" s="6" t="s">
         <v>7</v>
@@ -4272,12 +4268,12 @@
         <v>6</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
-      <c r="L71" s="17" t="s">
-        <v>21</v>
+      <c r="L71" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="M71" s="3" t="s">
         <v>3</v>
@@ -4285,12 +4281,10 @@
       <c r="N71" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O71" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P71" s="16" t="s">
-        <v>19</v>
-      </c>
+      <c r="O71" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P71" s="10"/>
       <c r="Q71" s="3"/>
       <c r="R71" s="3"/>
       <c r="S71" s="3"/>
@@ -4322,8 +4316,8 @@
       </c>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
-      <c r="L72" s="15" t="s">
-        <v>25</v>
+      <c r="L72" s="18" t="s">
+        <v>113</v>
       </c>
       <c r="M72" s="3" t="s">
         <v>3</v>
@@ -4331,17 +4325,17 @@
       <c r="N72" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O72" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P72" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q72" s="10"/>
-      <c r="R72" s="10"/>
-      <c r="S72" s="10"/>
-      <c r="T72" s="10"/>
-      <c r="U72" s="10"/>
+      <c r="O72" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P72" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q72" s="3"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="3"/>
+      <c r="T72" s="3"/>
+      <c r="U72" s="3"/>
       <c r="V72" s="2"/>
       <c r="W72" s="2"/>
       <c r="X72" s="3"/>
@@ -4355,7 +4349,7 @@
         <v>7</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G73" s="6" t="s">
         <v>7</v>
@@ -4368,8 +4362,8 @@
       </c>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
-      <c r="L73" s="12" t="s">
-        <v>4</v>
+      <c r="L73" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="M73" s="3" t="s">
         <v>3</v>
@@ -4377,17 +4371,17 @@
       <c r="N73" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O73" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P73" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q73" s="10"/>
-      <c r="R73" s="10"/>
-      <c r="S73" s="10"/>
-      <c r="T73" s="10"/>
-      <c r="U73" s="10"/>
+      <c r="O73" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P73" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="3"/>
+      <c r="T73" s="3"/>
+      <c r="U73" s="3"/>
       <c r="V73" s="2"/>
       <c r="W73" s="2"/>
       <c r="X73" s="3"/>
@@ -4401,7 +4395,7 @@
         <v>7</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G74" s="6" t="s">
         <v>7</v>
@@ -4410,12 +4404,12 @@
         <v>6</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
-      <c r="L74" s="12" t="s">
-        <v>23</v>
+      <c r="L74" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="M74" s="3" t="s">
         <v>3</v>
@@ -4424,9 +4418,11 @@
         <v>2</v>
       </c>
       <c r="O74" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P74" s="11"/>
+        <v>115</v>
+      </c>
+      <c r="P74" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="Q74" s="10"/>
       <c r="R74" s="10"/>
       <c r="S74" s="10"/>
@@ -4445,7 +4441,7 @@
         <v>7</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>7</v>
@@ -4468,10 +4464,10 @@
         <v>2</v>
       </c>
       <c r="O75" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P75" s="11" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="Q75" s="10"/>
       <c r="R75" s="10"/>
@@ -4480,7 +4476,7 @@
       <c r="U75" s="10"/>
       <c r="V75" s="2"/>
       <c r="W75" s="2"/>
-      <c r="X75" s="9"/>
+      <c r="X75" s="3"/>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
@@ -4491,7 +4487,7 @@
         <v>7</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G76" s="6" t="s">
         <v>7</v>
@@ -4500,12 +4496,12 @@
         <v>6</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
-      <c r="L76" s="18" t="s">
-        <v>114</v>
+      <c r="L76" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="M76" s="3" t="s">
         <v>3</v>
@@ -4513,20 +4509,18 @@
       <c r="N76" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O76" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P76" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q76" s="3"/>
-      <c r="R76" s="3"/>
-      <c r="S76" s="3"/>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
+      <c r="O76" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P76" s="11"/>
+      <c r="Q76" s="10"/>
+      <c r="R76" s="10"/>
+      <c r="S76" s="10"/>
+      <c r="T76" s="10"/>
+      <c r="U76" s="10"/>
       <c r="V76" s="2"/>
       <c r="W76" s="2"/>
-      <c r="X76" s="9"/>
+      <c r="X76" s="3"/>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
@@ -4537,7 +4531,7 @@
         <v>7</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G77" s="6" t="s">
         <v>7</v>
@@ -4550,8 +4544,8 @@
       </c>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
-      <c r="L77" s="17" t="s">
-        <v>21</v>
+      <c r="L77" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="M77" s="3" t="s">
         <v>3</v>
@@ -4559,17 +4553,17 @@
       <c r="N77" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O77" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P77" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q77" s="3"/>
-      <c r="R77" s="3"/>
-      <c r="S77" s="3"/>
-      <c r="T77" s="3"/>
-      <c r="U77" s="3"/>
+      <c r="O77" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P77" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q77" s="10"/>
+      <c r="R77" s="10"/>
+      <c r="S77" s="10"/>
+      <c r="T77" s="10"/>
+      <c r="U77" s="10"/>
       <c r="V77" s="2"/>
       <c r="W77" s="2"/>
       <c r="X77" s="9"/>
@@ -4583,7 +4577,7 @@
         <v>7</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G78" s="6" t="s">
         <v>7</v>
@@ -4592,12 +4586,12 @@
         <v>6</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
-      <c r="L78" s="15" t="s">
-        <v>17</v>
+      <c r="L78" s="18" t="s">
+        <v>113</v>
       </c>
       <c r="M78" s="3" t="s">
         <v>3</v>
@@ -4605,17 +4599,17 @@
       <c r="N78" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O78" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P78" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q78" s="10"/>
-      <c r="R78" s="10"/>
-      <c r="S78" s="10"/>
-      <c r="T78" s="10"/>
-      <c r="U78" s="10"/>
+      <c r="O78" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P78" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="3"/>
+      <c r="T78" s="3"/>
+      <c r="U78" s="3"/>
       <c r="V78" s="2"/>
       <c r="W78" s="2"/>
       <c r="X78" s="9"/>
@@ -4629,7 +4623,7 @@
         <v>7</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G79" s="6" t="s">
         <v>7</v>
@@ -4638,12 +4632,12 @@
         <v>6</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
-      <c r="L79" s="14" t="s">
-        <v>111</v>
+      <c r="L79" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="M79" s="3" t="s">
         <v>3</v>
@@ -4651,17 +4645,17 @@
       <c r="N79" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O79" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P79" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q79" s="10"/>
-      <c r="R79" s="10"/>
-      <c r="S79" s="10"/>
-      <c r="T79" s="10"/>
-      <c r="U79" s="10"/>
+      <c r="O79" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P79" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="3"/>
+      <c r="T79" s="3"/>
+      <c r="U79" s="3"/>
       <c r="V79" s="2"/>
       <c r="W79" s="2"/>
       <c r="X79" s="9"/>
@@ -4675,7 +4669,7 @@
         <v>7</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G80" s="6" t="s">
         <v>7</v>
@@ -4684,12 +4678,12 @@
         <v>6</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
-      <c r="L80" s="12" t="s">
-        <v>4</v>
+      <c r="L80" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="M80" s="3" t="s">
         <v>3</v>
@@ -4698,10 +4692,10 @@
         <v>2</v>
       </c>
       <c r="O80" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P80" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="Q80" s="10"/>
       <c r="R80" s="10"/>
@@ -4721,7 +4715,7 @@
         <v>7</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>7</v>
@@ -4730,12 +4724,12 @@
         <v>6</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
-      <c r="L81" s="35">
-        <v>1</v>
+      <c r="L81" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="M81" s="3" t="s">
         <v>3</v>
@@ -4743,13 +4737,17 @@
       <c r="N81" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O81" s="32"/>
-      <c r="P81" s="11"/>
-      <c r="Q81" s="32"/>
-      <c r="R81" s="32"/>
-      <c r="S81" s="32"/>
-      <c r="T81" s="32"/>
-      <c r="U81" s="32"/>
+      <c r="O81" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P81" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q81" s="10"/>
+      <c r="R81" s="10"/>
+      <c r="S81" s="10"/>
+      <c r="T81" s="10"/>
+      <c r="U81" s="10"/>
       <c r="V81" s="2"/>
       <c r="W81" s="2"/>
       <c r="X81" s="9"/>
@@ -4774,6 +4772,7 @@
       <c r="I82" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="J82" s="3"/>
       <c r="K82" s="3"/>
       <c r="L82" s="12" t="s">
         <v>4</v>
@@ -4784,17 +4783,17 @@
       <c r="N82" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O82" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="P82" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q82" s="11"/>
-      <c r="R82" s="11"/>
-      <c r="S82" s="11"/>
-      <c r="T82" s="11"/>
-      <c r="U82" s="11"/>
+      <c r="O82" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P82" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q82" s="10"/>
+      <c r="R82" s="10"/>
+      <c r="S82" s="10"/>
+      <c r="T82" s="10"/>
+      <c r="U82" s="10"/>
       <c r="V82" s="2"/>
       <c r="W82" s="2"/>
       <c r="X82" s="9"/>
@@ -4808,7 +4807,7 @@
         <v>7</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G83" s="6" t="s">
         <v>7</v>
@@ -4817,12 +4816,12 @@
         <v>6</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
-      <c r="L83" s="12" t="s">
-        <v>4</v>
+      <c r="L83" s="35">
+        <v>1</v>
       </c>
       <c r="M83" s="3" t="s">
         <v>3</v>
@@ -4830,20 +4829,16 @@
       <c r="N83" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O83" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P83" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q83" s="10"/>
-      <c r="R83" s="10"/>
-      <c r="S83" s="10"/>
-      <c r="T83" s="10"/>
-      <c r="U83" s="10"/>
+      <c r="O83" s="32"/>
+      <c r="P83" s="11"/>
+      <c r="Q83" s="32"/>
+      <c r="R83" s="32"/>
+      <c r="S83" s="32"/>
+      <c r="T83" s="32"/>
+      <c r="U83" s="32"/>
       <c r="V83" s="2"/>
       <c r="W83" s="2"/>
-      <c r="X83" s="3"/>
+      <c r="X83" s="9"/>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
@@ -4854,7 +4849,7 @@
         <v>7</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G84" s="6" t="s">
         <v>7</v>
@@ -4865,7 +4860,6 @@
       <c r="I84" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J84" s="3"/>
       <c r="K84" s="3"/>
       <c r="L84" s="12" t="s">
         <v>4</v>
@@ -4876,17 +4870,17 @@
       <c r="N84" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O84" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="P84" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q84" s="10"/>
-      <c r="R84" s="10"/>
-      <c r="S84" s="10"/>
-      <c r="T84" s="10"/>
-      <c r="U84" s="10"/>
+      <c r="O84" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P84" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q84" s="11"/>
+      <c r="R84" s="11"/>
+      <c r="S84" s="11"/>
+      <c r="T84" s="11"/>
+      <c r="U84" s="11"/>
       <c r="V84" s="2"/>
       <c r="W84" s="2"/>
       <c r="X84" s="9"/>
@@ -4900,7 +4894,7 @@
         <v>7</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G85" s="6" t="s">
         <v>7</v>
@@ -4923,10 +4917,10 @@
         <v>2</v>
       </c>
       <c r="O85" s="10" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="P85" s="11" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="Q85" s="10"/>
       <c r="R85" s="10"/>
@@ -4935,79 +4929,171 @@
       <c r="U85" s="10"/>
       <c r="V85" s="2"/>
       <c r="W85" s="2"/>
-      <c r="X85" s="9"/>
+      <c r="X85" s="3"/>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M86" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N86" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O86" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="P86" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q86" s="10"/>
+      <c r="R86" s="10"/>
+      <c r="S86" s="10"/>
+      <c r="T86" s="10"/>
+      <c r="U86" s="10"/>
+      <c r="V86" s="2"/>
+      <c r="W86" s="2"/>
+      <c r="X86" s="9"/>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M87" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N87" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O87" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P87" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q87" s="10"/>
+      <c r="R87" s="10"/>
+      <c r="S87" s="10"/>
+      <c r="T87" s="10"/>
+      <c r="U87" s="10"/>
+      <c r="V87" s="2"/>
+      <c r="W87" s="2"/>
+      <c r="X87" s="9"/>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="C88" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D86" s="8" t="s">
+      <c r="D88" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E86" s="7" t="s">
+      <c r="E88" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F86" s="6" t="s">
+      <c r="F88" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G86" s="6" t="s">
+      <c r="G88" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H86" s="5" t="s">
+      <c r="H88" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I86" s="4" t="s">
+      <c r="I88" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J86" s="3" t="s">
+      <c r="J88" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K86" s="3" t="s">
+      <c r="K88" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L86" s="3" t="s">
+      <c r="L88" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M86" s="3" t="s">
+      <c r="M88" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="N86" s="3" t="s">
+      <c r="N88" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="O86" s="3" t="s">
+      <c r="O88" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P86" s="2" t="s">
+      <c r="P88" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="Q86" s="2" t="s">
+      <c r="Q88" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R86" s="2" t="s">
+      <c r="R88" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="S86" s="2" t="s">
+      <c r="S88" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T86" s="2" t="s">
+      <c r="T88" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="U86" s="2" t="s">
+      <c r="U88" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="V86" s="2" t="s">
+      <c r="V88" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="W86" s="2" t="s">
+      <c r="W88" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="X86" s="2" t="s">
+      <c r="X88" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>